<commit_message>
New Commit perticular mail replay
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -36,11 +36,11 @@
   </si>
   <si>
     <t>Hello {0},
-&lt;br/&gt;
+&lt;br&gt;&lt;br&gt;
 we will get back to soon as per your mail
-&lt;br/&gt;
-Thank you! &lt;br/&gt;
-Chethan P</t>
+&lt;br&gt;&lt;br&gt;
+Thank you! &lt;br&gt;
+Chethan P&lt;br&gt;</t>
   </si>
 </sst>
 </file>

</xml_diff>